<commit_message>
xlsx distribution files for bar plots
</commit_message>
<xml_diff>
--- a/project_ECE/Geometry Garage.tsv.xlsx
+++ b/project_ECE/Geometry Garage.tsv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aspeake\Documents\OpenStudio-BuildStock\project_ECE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{40F57A07-AF07-49A7-B6B1-6898653781B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BDB4F-28D9-43AE-AAC1-6332D935953D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry Garage" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
   <si>
     <t>Dependency=Vintage</t>
   </si>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +411,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -572,8 +578,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -922,7 +929,338 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Geometry Garage'!$K$4:$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>&lt;1950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500-2499</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="dkUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-A2EC-4D54-A7E1-A7828122D113}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Geometry Garage'!$M$3:$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Car</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Car</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 Car</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Geometry Garage'!$M$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.82311779641500005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5726729243900004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6273259286500004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8822150544600004E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2EC-4D54-A7E1-A7828122D113}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="90"/>
+        <c:overlap val="-27"/>
+        <c:axId val="601277360"/>
+        <c:axId val="601282280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="601277360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601282280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="601282280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601277360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1465,6 +1803,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1498,6 +2339,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B75C969-0D75-4317-AE3D-6E0890F264FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1802,11 +2679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,22 +2779,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>7.5726729243900004E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>9.6273259286500004E-2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>4.8822150544600004E-3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.82311779641500005</v>
       </c>
       <c r="G3">
@@ -1925,6 +2802,18 @@
       </c>
       <c r="H3">
         <v>4207616.5596700003</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1952,6 +2841,24 @@
       <c r="H4">
         <v>1767455.92658</v>
       </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>0.82311779641500005</v>
+      </c>
+      <c r="N4">
+        <v>7.5726729243900004E-2</v>
+      </c>
+      <c r="O4">
+        <v>9.6273259286500004E-2</v>
+      </c>
+      <c r="P4">
+        <v>4.8822150544600004E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2214,22 +3121,22 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>0.109832447933</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>0.50216549429400004</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>2.8268843838000001E-2</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>0.35973321393399998</v>
       </c>
       <c r="G15">

</xml_diff>

<commit_message>
change distribution plots to percentage y axis
</commit_message>
<xml_diff>
--- a/project_ECE/Geometry Garage.tsv.xlsx
+++ b/project_ECE/Geometry Garage.tsv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aspeake\Documents\OpenStudio-BuildStock\project_ECE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BDB4F-28D9-43AE-AAC1-6332D935953D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097A0302-0693-4CD2-8E91-915BBFE8FE77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry Garage" sheetId="1" r:id="rId1"/>
@@ -842,7 +842,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1133,7 +1133,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2310,16 +2310,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2346,16 +2346,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>